<commit_message>
Splitted Makefile tasks into more Makefiles
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -416,7 +416,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20200120_110833</t>
+          <t>20200120_141715</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -931,667 +931,667 @@
     </row>
     <row r="2"/>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
       </c>
       <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3" t="n">
+        <v>9</v>
+      </c>
+      <c r="J3" t="n">
+        <v>9</v>
+      </c>
+      <c r="K3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.55034097</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5523893233333333</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8720895450372463</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.5489532422222223</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.5919831855555555</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.48116151</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.55165125</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.806262604818946</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.49165294</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.6631004700000001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.005716944262746474</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.01665251555453708</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2554508053313077</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.01266271277326345</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.03351250531299177</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.026002782784144</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0360965470677771</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.008421461227102094</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.02653895765541478</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.1078112559292301</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>0.54368234</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.5371520000000001</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.553272330933099</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="C6" t="n">
+        <v>0.53231406</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.7841679035111024</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.5222365</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.5860193</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.47300217</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.5729571999999999</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.8090142272975995</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.48541173</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.71755534</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.5523465999999999</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.5589866999999999</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.7895693771245247</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.5401235</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.61583084</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.46220303</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.5511644</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.8079969149171405</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.47341317</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.6780656999999999</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.54368234</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.55660003</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.7895497499390199</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.5469649000000001</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.5970192600000001</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.4600432</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.5361838000000001</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.8151036746816038</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.47369403</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.6438064999999999</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.55595666</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.55865896</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.7878517162928943</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.5598115299999999</v>
-      </c>
       <c r="F6" t="n">
-        <v>0.59512275</v>
+        <v>0.5486693</v>
       </c>
       <c r="G6" t="n">
         <v>0.45788336</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5333809</v>
+        <v>0.504023</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8110756272888595</v>
+        <v>0.7935657554002354</v>
       </c>
       <c r="J6" t="n">
         <v>0.4717893</v>
       </c>
       <c r="K6" t="n">
+        <v>0.4811514</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.54368234</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.53774</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.7855918256814729</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.5454463000000001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.5627826500000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.46220303</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.5333809</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.799738092633612</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.47369403</v>
+      </c>
+      <c r="K7" t="n">
         <v>0.63963985</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.55090255</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.55660003</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.7873124332204192</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.5514599</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.59512275</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.47300217</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.5511644</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.8079969149171405</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.48541173</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.6625951</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5530686</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.5589866999999999</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.7895497499390199</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.5545628</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.61583084</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.49028078</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.5654216999999999</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.8110756272888595</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.4936419</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.6885941</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.5595668</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.58252776</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.553272330933099</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.5661358</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.64200026</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.54211664</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.6290456999999999</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.8194355534683293</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.5585591999999999</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.8809408000000001</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>epoch,accuracy</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>f1_m</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>loss</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>precision_m</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>recall_m</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>val_accuracy</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>val_f1_m</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>val_loss</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>val_precision_m</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>val_recall_m</t>
+        </is>
+      </c>
+    </row>
+    <row r="14"/>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.54368234</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.5371520000000001</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.553272330933099</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.5222365</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5860193</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.47300217</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.5729571999999999</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.8090142272975995</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.48541173</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.71755534</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.5523465999999999</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.5589866999999999</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.7895693771245247</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.5401235</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.61583084</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.46220303</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.5511644</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.8079969149171405</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.47341317</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.6780656999999999</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.54368234</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.55660003</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.7895497499390199</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.5469649000000001</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.5970192600000001</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.4600432</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.5361838000000001</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.8151036746816038</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.47369403</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.6438064999999999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.55595666</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.55865896</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.7878517162928943</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.5598115299999999</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.59512275</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.45788336</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.5333809</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.8110756272888595</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.4717893</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.63963985</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>4</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B19" t="n">
         <v>0.5530686</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C19" t="n">
         <v>0.58252776</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D19" t="n">
         <v>0.7873124332204192</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E19" t="n">
         <v>0.55383795</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F19" t="n">
         <v>0.64200026</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G19" t="n">
         <v>0.4924406</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H19" t="n">
         <v>0.52085435</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I19" t="n">
         <v>0.8018057849700714</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J19" t="n">
         <v>0.49446672</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K19" t="n">
         <v>0.57555544</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="20">
+      <c r="A20" t="n">
         <v>5</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B20" t="n">
         <v>0.5595668</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C20" t="n">
         <v>0.5404206</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.7855918256814729</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.5661358</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.5627826500000001</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.49028078</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.6290456999999999</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.8194355534683293</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.4936419</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.8809408000000001</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.5501805000000001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.5671038</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.7868907463249317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.5454463000000001</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.62962544</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.54211664</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.504023</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.7935657554002354</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.5585591999999999</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.4811514</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.55090255</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.53774</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.7845998223077519</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.5545628</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.5486693</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.47300217</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.5518301999999999</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.7986278127130628</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.48437637</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.6625951</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.54368234</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.53231406</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.7841679035111024</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.5514599</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.55077887</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.47948164</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.5654216999999999</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.799738092633612</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.48952404</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.6885941</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>epoch,accuracy</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>f1_m</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>loss</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>precision_m</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>recall_m</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>val_accuracy</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>val_f1_m</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>val_loss</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>val_precision_m</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>val_recall_m</t>
-        </is>
-      </c>
-    </row>
-    <row r="15"/>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>count</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>9</v>
-      </c>
-      <c r="C16" t="n">
-        <v>9</v>
-      </c>
-      <c r="D16" t="n">
-        <v>9</v>
-      </c>
-      <c r="E16" t="n">
-        <v>9</v>
-      </c>
-      <c r="F16" t="n">
-        <v>9</v>
-      </c>
-      <c r="G16" t="n">
-        <v>9</v>
-      </c>
-      <c r="H16" t="n">
-        <v>9</v>
-      </c>
-      <c r="I16" t="n">
-        <v>9</v>
-      </c>
-      <c r="J16" t="n">
-        <v>9</v>
-      </c>
-      <c r="K16" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0.55034097</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.5523893233333333</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.8720895450372463</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.5489532422222223</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.5919831855555555</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.48116151</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.55165125</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.806262604818946</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.49165294</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.6631004700000001</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>std</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0.005716944262746474</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.01665251555453708</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.2554508053313077</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.01266271277326345</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.03351250531299177</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.026002782784144</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.0360965470677771</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.008421461227102094</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.02653895765541478</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.1078112559292301</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>min</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.54368234</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.53231406</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.7841679035111024</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.5222365</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.5486693</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.45788336</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.504023</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.7935657554002354</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.4717893</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0.4811514</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0.54368234</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.53774</v>
       </c>
       <c r="D20" t="n">
         <v>0.7855918256814729</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5454463000000001</v>
+        <v>0.5661358</v>
       </c>
       <c r="F20" t="n">
         <v>0.5627826500000001</v>
       </c>
       <c r="G20" t="n">
-        <v>0.46220303</v>
+        <v>0.49028078</v>
       </c>
       <c r="H20" t="n">
-        <v>0.5333809</v>
+        <v>0.6290456999999999</v>
       </c>
       <c r="I20" t="n">
-        <v>0.799738092633612</v>
+        <v>0.8194355534683293</v>
       </c>
       <c r="J20" t="n">
-        <v>0.47369403</v>
+        <v>0.4936419</v>
       </c>
       <c r="K20" t="n">
-        <v>0.63963985</v>
+        <v>0.8809408000000001</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>50%</t>
-        </is>
+      <c r="A21" t="n">
+        <v>6</v>
       </c>
       <c r="B21" t="n">
+        <v>0.5501805000000001</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.5671038</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.7868907463249317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.5454463000000001</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.62962544</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.54211664</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.504023</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.7935657554002354</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.5585591999999999</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.4811514</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>7</v>
+      </c>
+      <c r="B22" t="n">
         <v>0.55090255</v>
       </c>
-      <c r="C21" t="n">
-        <v>0.55660003</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.7873124332204192</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.5514599</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.59512275</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.47300217</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.5511644</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.8079969149171405</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0.48541173</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0.6625951</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.5530686</v>
-      </c>
       <c r="C22" t="n">
-        <v>0.5589866999999999</v>
+        <v>0.53774</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7895497499390199</v>
+        <v>0.7845998223077519</v>
       </c>
       <c r="E22" t="n">
         <v>0.5545628</v>
       </c>
       <c r="F22" t="n">
-        <v>0.61583084</v>
+        <v>0.5486693</v>
       </c>
       <c r="G22" t="n">
-        <v>0.49028078</v>
+        <v>0.47300217</v>
       </c>
       <c r="H22" t="n">
+        <v>0.5518301999999999</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.7986278127130628</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.48437637</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.6625951</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>8</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.54368234</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.53231406</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.7841679035111024</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.5514599</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.55077887</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.47948164</v>
+      </c>
+      <c r="H23" t="n">
         <v>0.5654216999999999</v>
       </c>
-      <c r="I22" t="n">
-        <v>0.8110756272888595</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0.4936419</v>
-      </c>
-      <c r="K22" t="n">
+      <c r="I23" t="n">
+        <v>0.799738092633612</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.48952404</v>
+      </c>
+      <c r="K23" t="n">
         <v>0.6885941</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>max</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>0.5595668</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.58252776</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1.553272330933099</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.5661358</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.64200026</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.54211664</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.6290456999999999</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0.8194355534683293</v>
-      </c>
-      <c r="J23" t="n">
-        <v>0.5585591999999999</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0.8809408000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added notebook for experiments via raw neural networks without using a custom class object
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -416,7 +416,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20200120_141715</t>
+          <t>20200121_101612</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -739,6 +739,16 @@
       </c>
     </row>
     <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>experimental_mode</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr">
         <is>
           <t>input_dim</t>

</xml_diff>